<commit_message>
UPDATE to sprint backlog
Caitlins updated her part in sprint backlog
</commit_message>
<xml_diff>
--- a/Sprint backlog.xlsx
+++ b/Sprint backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\computing\Desktop\Software-Engineering-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97D1A9C-8852-4D4B-92A8-052E00B765A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint backlog" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Sprint Planning</t>
   </si>
@@ -131,16 +132,31 @@
     <t>Hayden</t>
   </si>
   <si>
-    <t>Group Evaluation</t>
-  </si>
-  <si>
     <t>Sprint Chart Generator</t>
+  </si>
+  <si>
+    <t>Whole Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NA</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Caitlin / Sav</t>
+  </si>
+  <si>
+    <t>Caitlin/Sav</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,25 +511,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -532,7 +548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6" t="s">
@@ -547,7 +563,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>18</v>
@@ -558,7 +574,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>17</v>
@@ -566,14 +582,20 @@
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -581,14 +603,20 @@
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -596,14 +624,20 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>22</v>
@@ -611,14 +645,20 @@
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
@@ -629,7 +669,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -646,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -663,7 +703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -680,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -697,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -714,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>2</v>
@@ -725,7 +765,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -742,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -759,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -776,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -793,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -810,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>10</v>
       </c>
@@ -827,12 +867,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>34</v>
@@ -844,22 +884,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>27</v>
-      </c>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
+      <c r="G22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>